<commit_message>
commit databse + documentation
</commit_message>
<xml_diff>
--- a/documentation/3_1_Journal_Barras_Matias.xlsx
+++ b/documentation/3_1_Journal_Barras_Matias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/matias_barras_studentfr_ch/Documents/Dossier de formation/5-Modules/Développement/Module-306/306-G2-ArcadiaBox/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DA40C12-6F71-4A5C-9665-B8F6AA2F62EC}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6882072-E204-4185-BBBF-6A6EC1E20933}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Journal_Barras_Matias!$A$5:$HI$5</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Journal_Barras_Matias!$B:$D,Journal_Barras_Matias!$1:$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal_Barras_Matias!$A$1:$D$83</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal_Barras_Matias!$A$1:$D$85</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -126,13 +126,22 @@
     <t>Création du kanban</t>
   </si>
   <si>
-    <t>Kickof</t>
-  </si>
-  <si>
     <t>Début de la création de la structures de fichers</t>
   </si>
   <si>
     <t>Documentation sur les outils utillisé</t>
+  </si>
+  <si>
+    <t>Préparations des tâches du sprint (quoi faire, combien de temps)</t>
+  </si>
+  <si>
+    <t>Kick off</t>
+  </si>
+  <si>
+    <t>Documentation de Projet et shémas de la databse</t>
+  </si>
+  <si>
+    <t>Cette journée a été riche en documentation nous avons du décider quoi faire et comment et comprendre comment utilliser les outils que nous avons trouvé.</t>
   </si>
 </sst>
 </file>
@@ -429,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -572,6 +581,14 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1204,12 +1221,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EAF0F3-3EF4-4217-9640-9C9A8BC6D0F3}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft"/>
       <selection activeCell="A5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1332,7 +1349,9 @@
         <v>15</v>
       </c>
       <c r="C13" s="16"/>
-      <c r="D13" s="7"/>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
@@ -1340,68 +1359,86 @@
         <v>16</v>
       </c>
       <c r="C14" s="18"/>
-      <c r="D14" s="8"/>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="B15" s="17" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C15" s="18"/>
-      <c r="D15" s="8"/>
+      <c r="D15" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" s="18"/>
-      <c r="D16" s="8"/>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="D17" s="8"/>
+      <c r="D17" s="8">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="38"/>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="14"/>
+      <c r="B19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="8">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="14"/>
+      <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="9">
-        <f>SUM(D13:D17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="9">
+        <f>SUM(D13:D19)</f>
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="8"/>
+      <c r="B21" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="21"/>
+    </row>
+    <row r="22" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="13"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
@@ -1417,40 +1454,40 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="14"/>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="17"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="14"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="14"/>
+      <c r="B27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="9">
-        <f>SUM(D20:D24)</f>
+      <c r="D27" s="9">
+        <f>SUM(D22:D26)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
-    </row>
-    <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="8"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+    </row>
+    <row r="29" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="13"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="14"/>
@@ -1466,40 +1503,40 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="14"/>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="14"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="14"/>
+      <c r="B34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="9">
-        <f>SUM(D27:D31)</f>
+      <c r="D34" s="9">
+        <f>SUM(D29:D33)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="25"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
-    </row>
-    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="8"/>
+    <row r="35" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="25"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="24"/>
+    </row>
+    <row r="36" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="13"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="14"/>
@@ -1515,40 +1552,40 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="14"/>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="17"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="14"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="14"/>
+      <c r="B41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="9">
-        <f>SUM(D34:D38)</f>
+      <c r="D41" s="9">
+        <f>SUM(D36:D40)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="25"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="24"/>
-    </row>
-    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="13"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="7"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="8"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="8"/>
+    <row r="42" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="25"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="24"/>
+    </row>
+    <row r="43" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="13"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="7"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="14"/>
@@ -1564,40 +1601,40 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="14"/>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="17"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="14"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="14"/>
+      <c r="B48" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="9">
-        <f>SUM(D41:D45)</f>
+      <c r="D48" s="9">
+        <f>SUM(D43:D47)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="25"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="24"/>
-    </row>
-    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="13"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="7"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="8"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="14"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="8"/>
+    <row r="49" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="25"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="24"/>
+    </row>
+    <row r="50" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="13"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="7"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="14"/>
@@ -1613,40 +1650,40 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="14"/>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="17"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="14"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="14"/>
+      <c r="B55" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D53" s="9">
-        <f>SUM(D48:D52)</f>
+      <c r="D55" s="9">
+        <f>SUM(D50:D54)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="25"/>
-      <c r="B54" s="22"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="24"/>
-    </row>
-    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="13"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="7"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="14"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="8"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="8"/>
+    <row r="56" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="25"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="24"/>
+    </row>
+    <row r="57" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="13"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="7"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="14"/>
@@ -1662,40 +1699,40 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="14"/>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="17"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="8"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="14"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="8"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="14"/>
+      <c r="B62" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C62" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D60" s="9">
-        <f>SUM(D55:D59)</f>
+      <c r="D62" s="9">
+        <f>SUM(D57:D61)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="25"/>
-      <c r="B61" s="22"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="24"/>
-    </row>
-    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="13"/>
-      <c r="B62" s="15"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="7"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="14"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="8"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="14"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="18"/>
-      <c r="D64" s="8"/>
+    <row r="63" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="25"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="24"/>
+    </row>
+    <row r="64" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="13"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="7"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="14"/>
@@ -1711,40 +1748,40 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="14"/>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="17"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="8"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="14"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="8"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="14"/>
+      <c r="B69" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D67" s="9">
-        <f>SUM(D62:D66)</f>
+      <c r="D69" s="9">
+        <f>SUM(D64:D68)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="14"/>
-      <c r="B68" s="19"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="21"/>
-    </row>
-    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="13"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="16"/>
-      <c r="D69" s="7"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="14"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="8"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="14"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="8"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="21"/>
+    </row>
+    <row r="71" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="13"/>
+      <c r="B71" s="15"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="7"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="14"/>
@@ -1760,40 +1797,40 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="14"/>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="17"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="8"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="14"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="8"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="14"/>
+      <c r="B76" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D74" s="9">
-        <f>SUM(D69:D73)</f>
+      <c r="D76" s="9">
+        <f>SUM(D71:D75)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="25"/>
-      <c r="B75" s="22"/>
-      <c r="C75" s="23"/>
-      <c r="D75" s="24"/>
-    </row>
-    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="13"/>
-      <c r="B76" s="15"/>
-      <c r="C76" s="16"/>
-      <c r="D76" s="7"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="14"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="18"/>
-      <c r="D77" s="8"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="14"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="8"/>
+    <row r="77" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="25"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="24"/>
+    </row>
+    <row r="78" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="13"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="7"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="14"/>
@@ -1809,115 +1846,129 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="14"/>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="17"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="8"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="14"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="8"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="14"/>
+      <c r="B83" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C83" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D81" s="9">
-        <f>SUM(D76:D80)</f>
+      <c r="D83" s="9">
+        <f>SUM(D78:D82)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="25"/>
-      <c r="B82" s="22"/>
-      <c r="C82" s="23"/>
-      <c r="D82" s="24"/>
-    </row>
-    <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="11"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="3" t="s">
+    <row r="84" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="25"/>
+      <c r="B84" s="22"/>
+      <c r="C84" s="23"/>
+      <c r="D84" s="24"/>
+    </row>
+    <row r="85" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="11"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D83" s="12">
-        <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>3.4499999999999997</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="36" t="s">
+      <c r="D85" s="12">
+        <f>D11+D20+D27+D34+D41+D48+D55+D62+D69+D76+D83</f>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="36"/>
-      <c r="C84" s="36"/>
-      <c r="D84" s="36"/>
+      <c r="B86" s="36"/>
+      <c r="C86" s="36"/>
+      <c r="D86" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="82">
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
+  <mergeCells count="84">
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A78:A84"/>
     <mergeCell ref="B78:C78"/>
     <mergeCell ref="B79:C79"/>
     <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="A71:A77"/>
     <mergeCell ref="B71:C71"/>
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="A64:A70"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B65:C65"/>
     <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="A57:A63"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="A50:A56"/>
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="A43:A49"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="A36:A42"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="A29:A35"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="A22:A28"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="A13:A21"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B18:C18"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:A5"/>
@@ -1938,7 +1989,7 @@
       <formula>NOT(ISERROR(SEARCH("En cours",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:D18">
+  <conditionalFormatting sqref="D13:D20">
     <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D13)))</formula>
     </cfRule>
@@ -1946,84 +1997,84 @@
       <formula>NOT(ISERROR(SEARCH("En cours",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20:D25">
+  <conditionalFormatting sqref="D22:D27">
     <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D22)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="4" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D22)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D27:D32">
+  <conditionalFormatting sqref="D29:D34">
     <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D27)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D29)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D27)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D29)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34:D39">
+  <conditionalFormatting sqref="D36:D41">
     <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D34)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D36)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D34)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D36)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41:D46">
+  <conditionalFormatting sqref="D43:D48">
     <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D41)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D43)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D41)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D43)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48:D53">
+  <conditionalFormatting sqref="D50:D55">
     <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D48)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D50)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D48)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55:D60">
+  <conditionalFormatting sqref="D57:D62">
     <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D55)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D57)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D55)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D57)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D62:D67">
+  <conditionalFormatting sqref="D64:D69">
     <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D62)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="16" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D62)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D64)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D69:D74">
+  <conditionalFormatting sqref="D71:D76">
     <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D69)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D71)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D69)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D71)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D76:D81">
+  <conditionalFormatting sqref="D78:D83">
     <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D76)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D78)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D76)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D78)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D83">
+  <conditionalFormatting sqref="D85">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D83)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D85)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D83)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D85)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -2035,8 +2086,8 @@
     <oddFooter>&amp;L&amp;8&amp;F&amp;R&amp;8Page &amp;P/&amp;N</oddFooter>
   </headerFooter>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="47" max="16383" man="1"/>
-    <brk id="83" max="3" man="1"/>
+    <brk id="49" max="16383" man="1"/>
+    <brk id="85" max="3" man="1"/>
   </rowBreaks>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
routes des scores fonctionelle et containeriser
</commit_message>
<xml_diff>
--- a/documentation/3_1_Journal_Barras_Matias.xlsx
+++ b/documentation/3_1_Journal_Barras_Matias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/matias_barras_studentfr_ch/Documents/Dossier de formation/5-Modules/Développement/Module-306/306-G2-ArcadiaBox/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6882072-E204-4185-BBBF-6A6EC1E20933}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D383DBAA-5019-4FEA-BE83-BB5984A6000A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35520" yWindow="3000" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal_Barras_Matias" sheetId="10" r:id="rId1"/>
@@ -20,8 +20,11 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Journal_Barras_Matias!$B:$D,Journal_Barras_Matias!$1:$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Journal_Barras_Matias!$A$1:$D$85</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -29,6 +32,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,44 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
-  <si>
-    <t>Insérer les lignes au-dessus de celle-ci !</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Travail effectué</t>
-  </si>
-  <si>
-    <t>[H.h]</t>
-  </si>
-  <si>
-    <t>Temps</t>
-  </si>
-  <si>
-    <t>Total &gt;</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Réflexion personnelle </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>↓↓↓</t>
-    </r>
-  </si>
-  <si>
-    <t>[no candidat]</t>
-  </si>
-  <si>
-    <t>Total général &gt;</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <r>
       <t xml:space="preserve">Projet : </t>
@@ -108,6 +76,21 @@
     <t>Barras Matias</t>
   </si>
   <si>
+    <t>[no candidat]</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Travail effectué</t>
+  </si>
+  <si>
+    <t>Temps</t>
+  </si>
+  <si>
+    <t>[H.h]</t>
+  </si>
+  <si>
     <t>Documentation BusinessCase</t>
   </si>
   <si>
@@ -115,6 +98,22 @@
   </si>
   <si>
     <t>Discution client</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Réflexion personnelle </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>↓↓↓</t>
+    </r>
+  </si>
+  <si>
+    <t>Total &gt;</t>
   </si>
   <si>
     <t>Cette après-midi c'est bien passé mais faire de la documentation reste moin motivant que codée.</t>
@@ -126,22 +125,31 @@
     <t>Création du kanban</t>
   </si>
   <si>
+    <t>Kick off</t>
+  </si>
+  <si>
+    <t>Préparations des tâches du sprint (quoi faire, combien de temps)</t>
+  </si>
+  <si>
     <t>Début de la création de la structures de fichers</t>
   </si>
   <si>
     <t>Documentation sur les outils utillisé</t>
   </si>
   <si>
-    <t>Préparations des tâches du sprint (quoi faire, combien de temps)</t>
-  </si>
-  <si>
-    <t>Kick off</t>
-  </si>
-  <si>
     <t>Documentation de Projet et shémas de la databse</t>
   </si>
   <si>
     <t>Cette journée a été riche en documentation nous avons du décider quoi faire et comment et comprendre comment utilliser les outils que nous avons trouvé.</t>
+  </si>
+  <si>
+    <t>Total général &gt;</t>
+  </si>
+  <si>
+    <t>Insérer les lignes au-dessus de celle-ci !</t>
+  </si>
+  <si>
+    <t>Création du scripte pour extraire le texte et teste d'autres solution (écheque)</t>
   </si>
 </sst>
 </file>
@@ -487,14 +495,74 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -504,23 +572,15 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -535,60 +595,8 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -871,6 +879,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1223,10 +1235,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EAF0F3-3EF4-4217-9640-9C9A8BC6D0F3}">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft"/>
       <selection activeCell="A5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1239,94 +1251,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
+      <c r="A2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20">
+        <v>45996</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26">
-        <v>45996</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="7">
         <v>1.8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="18"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="25"/>
       <c r="D7" s="8">
         <v>1.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="18"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="25"/>
       <c r="D8" s="8">
         <v>0.15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D11" s="9">
         <f>SUM(D6:D10)</f>
@@ -1334,92 +1346,92 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13">
+      <c r="A13" s="29">
         <v>46003</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="16"/>
+      <c r="B13" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="31"/>
       <c r="D13" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="18"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="25"/>
       <c r="D14" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="18"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="25"/>
       <c r="D15" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="18"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="25"/>
       <c r="D16" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="17" t="s">
+      <c r="A17" s="21"/>
+      <c r="B17" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="18"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="8">
         <v>0.25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="37" t="s">
+      <c r="A18" s="21"/>
+      <c r="B18" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="38"/>
+      <c r="C18" s="33"/>
       <c r="D18" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="18"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="25"/>
       <c r="D19" s="8">
         <v>3.2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D20" s="9">
         <f>SUM(D13:D19)</f>
@@ -1427,99 +1439,103 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="21"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
     </row>
     <row r="22" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="7"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="31"/>
+      <c r="D22" s="7">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="25"/>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="8"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D27" s="9">
         <f>SUM(D22:D26)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="21"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="28"/>
     </row>
     <row r="29" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="16"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="31"/>
       <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="18"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
       <c r="D32" s="8"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="14"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="18"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
       <c r="D33" s="8"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="14"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D34" s="9">
         <f>SUM(D29:D33)</f>
@@ -1527,48 +1543,48 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="25"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="24"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="37"/>
     </row>
     <row r="36" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="13"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="16"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="31"/>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="18"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="25"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="18"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="25"/>
       <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="14"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="18"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="25"/>
       <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="14"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D41" s="9">
         <f>SUM(D36:D40)</f>
@@ -1576,48 +1592,48 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="25"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="24"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="37"/>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="13"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="16"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="31"/>
       <c r="D43" s="7"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="18"/>
+      <c r="A44" s="21"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="25"/>
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="18"/>
+      <c r="A45" s="21"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="25"/>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="18"/>
+      <c r="A46" s="21"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="25"/>
       <c r="D46" s="8"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="14"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="18"/>
+      <c r="A47" s="21"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="25"/>
       <c r="D47" s="8"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="14"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D48" s="9">
         <f>SUM(D43:D47)</f>
@@ -1625,48 +1641,48 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="25"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="24"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="37"/>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="13"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="16"/>
+      <c r="A50" s="29"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="31"/>
       <c r="D50" s="7"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="14"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="18"/>
+      <c r="A51" s="21"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="25"/>
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="18"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="25"/>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="14"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="18"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="25"/>
       <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="14"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="18"/>
+      <c r="A54" s="21"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="25"/>
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="14"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D55" s="9">
         <f>SUM(D50:D54)</f>
@@ -1674,48 +1690,48 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="25"/>
-      <c r="B56" s="22"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="24"/>
+      <c r="A56" s="34"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="37"/>
     </row>
     <row r="57" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="13"/>
-      <c r="B57" s="15"/>
-      <c r="C57" s="16"/>
+      <c r="A57" s="29"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="31"/>
       <c r="D57" s="7"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="18"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="25"/>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="14"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="18"/>
+      <c r="A59" s="21"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="25"/>
       <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="14"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="18"/>
+      <c r="A60" s="21"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="25"/>
       <c r="D60" s="8"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="14"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="18"/>
+      <c r="A61" s="21"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="25"/>
       <c r="D61" s="8"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="14"/>
+      <c r="A62" s="21"/>
       <c r="B62" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D62" s="9">
         <f>SUM(D57:D61)</f>
@@ -1723,48 +1739,48 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="25"/>
-      <c r="B63" s="22"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="24"/>
+      <c r="A63" s="34"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="37"/>
     </row>
     <row r="64" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="13"/>
-      <c r="B64" s="15"/>
-      <c r="C64" s="16"/>
+      <c r="A64" s="29"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="31"/>
       <c r="D64" s="7"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="14"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="18"/>
+      <c r="A65" s="21"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="25"/>
       <c r="D65" s="8"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="14"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="18"/>
+      <c r="A66" s="21"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="25"/>
       <c r="D66" s="8"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="14"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="18"/>
+      <c r="A67" s="21"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="25"/>
       <c r="D67" s="8"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="14"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="18"/>
+      <c r="A68" s="21"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="25"/>
       <c r="D68" s="8"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="14"/>
+      <c r="A69" s="21"/>
       <c r="B69" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D69" s="9">
         <f>SUM(D64:D68)</f>
@@ -1772,48 +1788,48 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="14"/>
-      <c r="B70" s="19"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="21"/>
+      <c r="A70" s="21"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="28"/>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="13"/>
-      <c r="B71" s="15"/>
-      <c r="C71" s="16"/>
+      <c r="A71" s="29"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="31"/>
       <c r="D71" s="7"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="14"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="18"/>
+      <c r="A72" s="21"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="25"/>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="14"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="18"/>
+      <c r="A73" s="21"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="25"/>
       <c r="D73" s="8"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="14"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="18"/>
+      <c r="A74" s="21"/>
+      <c r="B74" s="24"/>
+      <c r="C74" s="25"/>
       <c r="D74" s="8"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="14"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="18"/>
+      <c r="A75" s="21"/>
+      <c r="B75" s="24"/>
+      <c r="C75" s="25"/>
       <c r="D75" s="8"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="14"/>
+      <c r="A76" s="21"/>
       <c r="B76" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D76" s="9">
         <f>SUM(D71:D75)</f>
@@ -1821,48 +1837,48 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="25"/>
-      <c r="B77" s="22"/>
-      <c r="C77" s="23"/>
-      <c r="D77" s="24"/>
+      <c r="A77" s="34"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="36"/>
+      <c r="D77" s="37"/>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="13"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="16"/>
+      <c r="A78" s="29"/>
+      <c r="B78" s="30"/>
+      <c r="C78" s="31"/>
       <c r="D78" s="7"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="14"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="18"/>
+      <c r="A79" s="21"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="25"/>
       <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="14"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="18"/>
+      <c r="A80" s="21"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="25"/>
       <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="14"/>
-      <c r="B81" s="17"/>
-      <c r="C81" s="18"/>
+      <c r="A81" s="21"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="25"/>
       <c r="D81" s="8"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="14"/>
-      <c r="B82" s="17"/>
-      <c r="C82" s="18"/>
+      <c r="A82" s="21"/>
+      <c r="B82" s="24"/>
+      <c r="C82" s="25"/>
       <c r="D82" s="8"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="14"/>
+      <c r="A83" s="21"/>
       <c r="B83" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D83" s="9">
         <f>SUM(D78:D82)</f>
@@ -1870,29 +1886,29 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="25"/>
-      <c r="B84" s="22"/>
-      <c r="C84" s="23"/>
-      <c r="D84" s="24"/>
+      <c r="A84" s="34"/>
+      <c r="B84" s="35"/>
+      <c r="C84" s="36"/>
+      <c r="D84" s="37"/>
     </row>
     <row r="85" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="11"/>
       <c r="B85" s="10"/>
       <c r="C85" s="3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D85" s="12">
         <f>D11+D20+D27+D34+D41+D48+D55+D62+D69+D76+D83</f>
-        <v>11.4</v>
+        <v>18.399999999999999</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B86" s="36"/>
-      <c r="C86" s="36"/>
-      <c r="D86" s="36"/>
+      <c r="A86" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B86" s="38"/>
+      <c r="C86" s="38"/>
+      <c r="D86" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="84">
@@ -2094,6 +2110,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3865b25f2bf2a035dbe7787239b3f11c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="718f9f7ddd2530d56a17ab9424d0abda" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -2306,7 +2331,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
@@ -2317,16 +2342,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2345,23 +2369,13 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
-    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
     <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
     <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
db simplifier et fonctionnelle avec les routes adaptées
</commit_message>
<xml_diff>
--- a/documentation/3_1_Journal_Barras_Matias.xlsx
+++ b/documentation/3_1_Journal_Barras_Matias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/matias_barras_studentfr_ch/Documents/Dossier de formation/5-Modules/Développement/Module-306/306-G2-ArcadiaBox/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D383DBAA-5019-4FEA-BE83-BB5984A6000A}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A8252C1-D818-4050-AD15-B17E92B420CC}"/>
   <bookViews>
-    <workbookView xWindow="35520" yWindow="3000" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal_Barras_Matias" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <r>
       <t xml:space="preserve">Projet : </t>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>Création du scripte pour extraire le texte et teste d'autres solution (écheque)</t>
+  </si>
+  <si>
+    <t>Création des dockerfiles ajout dans le docker compose et créations des routes du backend</t>
+  </si>
+  <si>
+    <t>Documentation et tests</t>
+  </si>
+  <si>
+    <t>Ce sprint a été très dure un début avec beaucoup de tests non concluant ce qui n'était pas très motivant cel a été emplifier du fait que j'était malade mais une fois la solution trouvé j'ai pu m'attaquer a des choses plus "tranquille" ce qui a été mieux</t>
   </si>
 </sst>
 </file>
@@ -495,6 +504,70 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -527,76 +600,12 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1236,9 +1245,9 @@
   <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B14" zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft"/>
       <selection activeCell="A5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22:C22"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1251,89 +1260,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="18"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="19"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20">
+      <c r="A6" s="36">
         <v>45996</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="23"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="7">
         <v>1.8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="24" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="25"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="8">
         <v>1.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
-      <c r="B8" s="24" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="25"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="8">
         <v>0.15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1346,87 +1355,87 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="26" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29">
+      <c r="A13" s="14">
         <v>46003</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="31"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
-      <c r="B14" s="24" t="s">
+      <c r="A14" s="15"/>
+      <c r="B14" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="25"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
-      <c r="B15" s="24" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="25"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="21"/>
-      <c r="B16" s="24" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="25"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
-      <c r="B17" s="24" t="s">
+      <c r="A17" s="15"/>
+      <c r="B17" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="25"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="8">
         <v>0.25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
-      <c r="B18" s="32" t="s">
+      <c r="A18" s="15"/>
+      <c r="B18" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="33"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="21"/>
-      <c r="B19" s="24" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="25"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="8">
         <v>3.2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="21"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="2" t="s">
         <v>10</v>
       </c>
@@ -1439,49 +1448,57 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
-      <c r="B21" s="26" t="s">
+      <c r="A21" s="15"/>
+      <c r="B21" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="28"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
     </row>
     <row r="22" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="30" t="s">
+      <c r="A22" s="14"/>
+      <c r="B22" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="31"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="7">
-        <v>7</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="8"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="8"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="8">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="25"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="8"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="21"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="2" t="s">
         <v>10</v>
       </c>
@@ -1490,47 +1507,49 @@
       </c>
       <c r="D27" s="9">
         <f>SUM(D22:D26)</f>
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="21"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="28"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
     </row>
     <row r="29" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="29"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="31"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
       <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="21"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="21"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="21"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="8"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="21"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
       <c r="D33" s="8"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="21"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="2" t="s">
         <v>10</v>
       </c>
@@ -1543,43 +1562,43 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="34"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="37"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="23"/>
     </row>
     <row r="36" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="29"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="31"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="21"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="25"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="21"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="25"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="21"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="25"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="20"/>
       <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="21"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="25"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="20"/>
       <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="21"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="2" t="s">
         <v>10</v>
       </c>
@@ -1592,43 +1611,43 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="34"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="37"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="23"/>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="29"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="31"/>
+      <c r="A43" s="14"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
       <c r="D43" s="7"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="21"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="25"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="20"/>
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="21"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="25"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="20"/>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="21"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="25"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="20"/>
       <c r="D46" s="8"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="21"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="25"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="20"/>
       <c r="D47" s="8"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="21"/>
+      <c r="A48" s="15"/>
       <c r="B48" s="2" t="s">
         <v>10</v>
       </c>
@@ -1641,43 +1660,43 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="34"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="37"/>
+      <c r="A49" s="16"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="23"/>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="29"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="31"/>
+      <c r="A50" s="14"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
       <c r="D50" s="7"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="21"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="25"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="20"/>
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="21"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="25"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="20"/>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="21"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="25"/>
+      <c r="A53" s="15"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="20"/>
       <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="21"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="25"/>
+      <c r="A54" s="15"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="20"/>
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="21"/>
+      <c r="A55" s="15"/>
       <c r="B55" s="2" t="s">
         <v>10</v>
       </c>
@@ -1690,43 +1709,43 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="34"/>
-      <c r="B56" s="35"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="37"/>
+      <c r="A56" s="16"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="23"/>
     </row>
     <row r="57" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="29"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="31"/>
+      <c r="A57" s="14"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
       <c r="D57" s="7"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="21"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="25"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="20"/>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="21"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="25"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="20"/>
       <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="21"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="25"/>
+      <c r="A60" s="15"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="20"/>
       <c r="D60" s="8"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="21"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="25"/>
+      <c r="A61" s="15"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="20"/>
       <c r="D61" s="8"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="21"/>
+      <c r="A62" s="15"/>
       <c r="B62" s="2" t="s">
         <v>10</v>
       </c>
@@ -1739,43 +1758,43 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="34"/>
-      <c r="B63" s="35"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="37"/>
+      <c r="A63" s="16"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="23"/>
     </row>
     <row r="64" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="29"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="31"/>
+      <c r="A64" s="14"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="18"/>
       <c r="D64" s="7"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="21"/>
-      <c r="B65" s="24"/>
-      <c r="C65" s="25"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="20"/>
       <c r="D65" s="8"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="21"/>
-      <c r="B66" s="24"/>
-      <c r="C66" s="25"/>
+      <c r="A66" s="15"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="20"/>
       <c r="D66" s="8"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="21"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="25"/>
+      <c r="A67" s="15"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="20"/>
       <c r="D67" s="8"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="21"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="25"/>
+      <c r="A68" s="15"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="20"/>
       <c r="D68" s="8"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="21"/>
+      <c r="A69" s="15"/>
       <c r="B69" s="2" t="s">
         <v>10</v>
       </c>
@@ -1788,43 +1807,43 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="21"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="27"/>
-      <c r="D70" s="28"/>
+      <c r="A70" s="15"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="25"/>
+      <c r="D70" s="26"/>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="29"/>
-      <c r="B71" s="30"/>
-      <c r="C71" s="31"/>
+      <c r="A71" s="14"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="18"/>
       <c r="D71" s="7"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="21"/>
-      <c r="B72" s="24"/>
-      <c r="C72" s="25"/>
+      <c r="A72" s="15"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="20"/>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="21"/>
-      <c r="B73" s="24"/>
-      <c r="C73" s="25"/>
+      <c r="A73" s="15"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="20"/>
       <c r="D73" s="8"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="21"/>
-      <c r="B74" s="24"/>
-      <c r="C74" s="25"/>
+      <c r="A74" s="15"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="20"/>
       <c r="D74" s="8"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="21"/>
-      <c r="B75" s="24"/>
-      <c r="C75" s="25"/>
+      <c r="A75" s="15"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="20"/>
       <c r="D75" s="8"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="21"/>
+      <c r="A76" s="15"/>
       <c r="B76" s="2" t="s">
         <v>10</v>
       </c>
@@ -1837,43 +1856,43 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="34"/>
-      <c r="B77" s="35"/>
-      <c r="C77" s="36"/>
-      <c r="D77" s="37"/>
+      <c r="A77" s="16"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="22"/>
+      <c r="D77" s="23"/>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="29"/>
-      <c r="B78" s="30"/>
-      <c r="C78" s="31"/>
+      <c r="A78" s="14"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="18"/>
       <c r="D78" s="7"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="21"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="25"/>
+      <c r="A79" s="15"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="20"/>
       <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="21"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="25"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="20"/>
       <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="21"/>
-      <c r="B81" s="24"/>
-      <c r="C81" s="25"/>
+      <c r="A81" s="15"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="20"/>
       <c r="D81" s="8"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="21"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="25"/>
+      <c r="A82" s="15"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="20"/>
       <c r="D82" s="8"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="21"/>
+      <c r="A83" s="15"/>
       <c r="B83" s="2" t="s">
         <v>10</v>
       </c>
@@ -1886,10 +1905,10 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="34"/>
-      <c r="B84" s="35"/>
-      <c r="C84" s="36"/>
-      <c r="D84" s="37"/>
+      <c r="A84" s="16"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="23"/>
     </row>
     <row r="85" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="11"/>
@@ -1899,92 +1918,19 @@
       </c>
       <c r="D85" s="12">
         <f>D11+D20+D27+D34+D41+D48+D55+D62+D69+D76+D83</f>
-        <v>18.399999999999999</v>
+        <v>23.4</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="38" t="s">
+      <c r="A86" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B86" s="38"/>
-      <c r="C86" s="38"/>
-      <c r="D86" s="38"/>
+      <c r="B86" s="13"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="A86:D86"/>
-    <mergeCell ref="A78:A84"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="A71:A77"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B77:D77"/>
-    <mergeCell ref="A64:A70"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="A57:A63"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="A50:A56"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="A43:A49"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="A36:A42"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:A5"/>
@@ -1996,6 +1942,79 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="A36:A42"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="A43:A49"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="A57:A63"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="A64:A70"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="A71:A77"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A78:A84"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B84:D84"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Terminé">
@@ -2110,15 +2129,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3865b25f2bf2a035dbe7787239b3f11c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="718f9f7ddd2530d56a17ab9424d0abda" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -2331,6 +2341,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2343,14 +2362,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2369,6 +2380,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
   <ds:schemaRefs>

</xml_diff>